<commit_message>
updating performance raw data
</commit_message>
<xml_diff>
--- a/performance_comparison_20200902.xlsx
+++ b/performance_comparison_20200902.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyongki/Documents/aws-projects/DDB_Query_Insight_ServerSide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA97D14A-AF65-E141-9ADE-B86B7B551189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CAEBAE-3640-C84B-B758-926EFB725720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16140" xr2:uid="{4D297C2A-EAAD-B643-8F2F-61B0F4F7675D}"/>
+    <workbookView xWindow="10820" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{4D297C2A-EAAD-B643-8F2F-61B0F4F7675D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <dimension ref="A2:I103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,7 +437,7 @@
         <v>47</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>51</v>
@@ -479,7 +479,7 @@
         <v>47</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>28</v>
@@ -500,7 +500,7 @@
         <v>52</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>34</v>
@@ -521,7 +521,7 @@
         <v>47</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -542,7 +542,7 @@
         <v>48</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>33</v>
@@ -563,7 +563,7 @@
         <v>57</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>35</v>
@@ -584,7 +584,7 @@
         <v>47</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>49</v>
@@ -605,7 +605,7 @@
         <v>49</v>
       </c>
       <c r="B11">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>31</v>
@@ -626,7 +626,7 @@
         <v>49</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>34</v>
@@ -649,7 +649,7 @@
       </c>
       <c r="B13">
         <f>AVERAGE(B3:B12)</f>
-        <v>11</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C13">
         <f>AVERAGE(C3:C12)</f>

</xml_diff>